<commit_message>
adding fuel flow from T2 document to the Databank and add engine fan area for turbofan engines and then the calculated mass flow to later determine thermal and propulsive efficiency
</commit_message>
<xml_diff>
--- a/overall/output/ovr_efficiency.xlsx
+++ b/overall/output/ovr_efficiency.xlsx
@@ -683,7 +683,7 @@
         <v>1989</v>
       </c>
       <c r="C19" t="n">
-        <v>1.493118904858319</v>
+        <v>1.493065291990434</v>
       </c>
     </row>
     <row r="20">
@@ -722,7 +722,7 @@
         <v>1995</v>
       </c>
       <c r="C22" t="n">
-        <v>1.392219378292582</v>
+        <v>1.392164305643596</v>
       </c>
     </row>
   </sheetData>
@@ -1070,7 +1070,7 @@
         <v>1995</v>
       </c>
       <c r="C25" t="n">
-        <v>1.339423267681455</v>
+        <v>1.340189934684793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>